<commit_message>
EPBDS-8616 Add more tests for ternary operation
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8616_ternary_operators.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8616_ternary_operators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diana\.openl\user-workspace\admin\test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37B5F94-DB10-4B00-992D-7DA889C4E432}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EBE9B1-9B31-4DAE-ADD5-37F91E7459B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5B8DFB6-0CD7-4287-8A9A-13C9212B465F}"/>
+    <workbookView xWindow="1320" yWindow="510" windowWidth="26400" windowHeight="13455" xr2:uid="{B5B8DFB6-0CD7-4287-8A9A-13C9212B465F}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>X</t>
   </si>
@@ -115,9 +115,6 @@
     <t>x3</t>
   </si>
   <si>
-    <t>Spreadsheet SpreadsheetResult ternaryOperators(Boolean b)</t>
-  </si>
-  <si>
     <t>= (b)?"t":"f"</t>
   </si>
   <si>
@@ -146,19 +143,117 @@
   </si>
   <si>
     <t>_res_.$x5.$x1</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>IsGood</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Boolean abc</t>
+  </si>
+  <si>
+    <t>SmartRules Double MyRule (Boolean abc, Integer Age)</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>(abc)?"good"</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult ternaryOperators(Boolean a, Boolean b)</t>
+  </si>
+  <si>
+    <t>= (a?b)?"c"</t>
+  </si>
+  <si>
+    <t>&lt;20</t>
+  </si>
+  <si>
+    <t>_res_.$x7</t>
+  </si>
+  <si>
+    <t>x7</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Test ternaryOperators ternaryOperatorsTest2</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Test MyRule MyRuleTest</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Abc</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&lt;=50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -173,15 +268,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -204,30 +305,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent1 10" xfId="2" xr:uid="{4D088DAB-C97B-4B03-80B1-0133679E92FC}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{7C0D6CA1-A13C-492C-B22E-2E894B518D97}"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{1E28F813-D77D-488A-8349-3DF49C674B8D}"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{826D6C58-A5AA-4505-9CE6-5D7E620BD896}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -240,9 +411,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -280,7 +451,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -386,7 +557,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -536,71 +707,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080FA793-3F28-4BB3-9382-CB32EE3B2341}">
-  <dimension ref="B3:K20"/>
+  <dimension ref="B3:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.5546875" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>2</v>
+      <c r="F5" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>2</v>
@@ -617,146 +788,356 @@
       <c r="K5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
+      <c r="L5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>8</v>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2">
+      <c r="H6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
         <v>10</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="D7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2" t="s">
+      <c r="D8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="J11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
+      <c r="K12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="J13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="J14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
+      <c r="G15" s="15"/>
+      <c r="J15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
+      <c r="J16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+      <c r="J17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="F26" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="16"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="13">
+        <v>2</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="13">
+        <v>7</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="14">
+        <v>40</v>
+      </c>
+      <c r="D42" s="14">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E15:F15"/>
+  <mergeCells count="5">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="B38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -766,7 +1147,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>